<commit_message>
update bom with selected parts
</commit_message>
<xml_diff>
--- a/FlashlightBOM.xlsx
+++ b/FlashlightBOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
   <si>
     <t>Top pcb</t>
   </si>
@@ -32,9 +32,6 @@
     <t>Bottom pcb</t>
   </si>
   <si>
-    <t>Resistor</t>
-  </si>
-  <si>
     <t>Switch</t>
   </si>
   <si>
@@ -126,6 +123,9 @@
   </si>
   <si>
     <t xml:space="preserve">or http://www.dx.com/p/aluminum-smooth-flashlight-reflector-silver-106488#.VC76FZ54rw9 </t>
+  </si>
+  <si>
+    <t>Regulator</t>
   </si>
 </sst>
 </file>
@@ -133,10 +133,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,6 +148,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -191,15 +198,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,366 +491,396 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" style="6" customWidth="1"/>
+    <col min="2" max="5" width="9.140625" style="6"/>
+    <col min="6" max="6" width="12.28515625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7">
+        <f>4.55/3</f>
+        <v>1.5166666666666666</v>
+      </c>
+      <c r="D2" s="8">
+        <f>C2*B2</f>
+        <v>1.5166666666666666</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7">
+        <f>4.55/3</f>
+        <v>1.5166666666666666</v>
+      </c>
+      <c r="D3" s="8">
+        <f>C3*B3</f>
+        <v>1.5166666666666666</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="6">
+        <f>4.55/3</f>
+        <v>1.5166666666666666</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7">
+        <f>11.09/100</f>
+        <v>0.1109</v>
+      </c>
+      <c r="D4" s="8">
+        <f t="shared" ref="D4:D12" si="0">C4*B4</f>
+        <v>0.1109</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="9">
+        <v>1124300</v>
+      </c>
+      <c r="M4" s="7">
+        <f>C2-M3</f>
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7">
-        <v>2.88</v>
-      </c>
-      <c r="D2" s="4">
-        <f>C2*B2</f>
-        <v>2.88</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7">
-        <v>2.88</v>
-      </c>
-      <c r="D3" s="4">
-        <f>C3*B3</f>
-        <v>2.88</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="D4" s="4">
-        <f t="shared" ref="D4:D12" si="0">C4*B4</f>
-        <v>0.2</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
+      <c r="B5" s="6">
         <v>1</v>
       </c>
       <c r="C5" s="7">
         <v>1.76</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="8">
         <f t="shared" si="0"/>
         <v>1.76</v>
       </c>
-      <c r="F5" t="s">
-        <v>18</v>
+      <c r="F5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="M5" s="6">
+        <f>M4*2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="D6" s="8">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" s="7">
-        <v>0.75</v>
-      </c>
-      <c r="D6" s="4">
-        <f t="shared" si="0"/>
-        <v>0.75</v>
-      </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7">
+      <c r="B7" s="6">
         <v>150</v>
       </c>
       <c r="C7" s="7">
         <f>1.88/(2*12*25.4)</f>
         <v>3.0839895013123363E-3</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="8">
         <f t="shared" si="0"/>
         <v>0.46259842519685046</v>
       </c>
-      <c r="F7" t="s">
-        <v>19</v>
+      <c r="F7" s="6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8">
+      <c r="A8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="6">
         <v>170</v>
       </c>
       <c r="C8" s="7">
         <f>2.95/15240</f>
         <v>1.9356955380577429E-4</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="8">
         <f t="shared" si="0"/>
         <v>3.2906824146981629E-2</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G8" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
+      <c r="A9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="6">
         <v>1</v>
       </c>
       <c r="C9" s="7">
         <v>0.46</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="8">
         <f t="shared" si="0"/>
         <v>0.46</v>
       </c>
-      <c r="F9" t="s">
-        <v>19</v>
+      <c r="F9" s="6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10">
+      <c r="A10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="6">
         <v>1</v>
       </c>
       <c r="C10" s="7">
         <v>0.76</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="8">
         <f t="shared" si="0"/>
         <v>0.76</v>
       </c>
-      <c r="F10" t="s">
-        <v>20</v>
-      </c>
-      <c r="I10" t="s">
-        <v>33</v>
+      <c r="F10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="6">
+        <v>1209700</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11">
+      <c r="A11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="6">
         <v>1</v>
       </c>
       <c r="C11" s="7">
         <v>0.122</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="8">
         <f t="shared" si="0"/>
         <v>0.122</v>
       </c>
-      <c r="F11" t="s">
-        <v>20</v>
+      <c r="F11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="6">
+        <v>1347100</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12">
+      <c r="A12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="6">
         <v>2</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="8">
         <v>0.113</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="8">
         <f t="shared" si="0"/>
         <v>0.22600000000000001</v>
       </c>
-      <c r="F12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" t="s">
-        <v>26</v>
-      </c>
-      <c r="L12" t="s">
+      <c r="F12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M12" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="N12" t="s">
-        <v>26</v>
-      </c>
-      <c r="O12">
+      <c r="O12" s="6">
         <v>0.113</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
     </row>
     <row r="15" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" s="2"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6">
+      <c r="C15" s="4"/>
+      <c r="D15" s="5">
         <f>SUM(D2:D14)</f>
-        <v>10.533505249343833</v>
+        <v>7.6677385826771642</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S16">
+      <c r="S16" s="6">
         <v>4.5</v>
       </c>
     </row>
     <row r="18" spans="12:23" x14ac:dyDescent="0.25">
-      <c r="L18" t="s">
-        <v>4</v>
-      </c>
-      <c r="M18" t="s">
-        <v>25</v>
-      </c>
-      <c r="N18" t="s">
-        <v>27</v>
-      </c>
-      <c r="O18">
+      <c r="L18" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="M18" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N18" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="O18" s="6">
         <v>0.78</v>
       </c>
-      <c r="Q18">
+      <c r="Q18" s="6">
         <v>2.95</v>
       </c>
-      <c r="R18">
+      <c r="R18" s="6">
         <v>350</v>
       </c>
-      <c r="S18">
+      <c r="S18" s="6">
         <f>($S$16-Q18)/(R18/1000)</f>
         <v>4.4285714285714279</v>
       </c>
-      <c r="V18" t="s">
-        <v>30</v>
-      </c>
-      <c r="W18">
+      <c r="V18" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="W18" s="6">
         <v>0.17699999999999999</v>
       </c>
     </row>
     <row r="19" spans="12:23" x14ac:dyDescent="0.25">
-      <c r="M19" t="s">
-        <v>25</v>
-      </c>
-      <c r="N19" t="s">
-        <v>28</v>
-      </c>
-      <c r="O19">
+      <c r="M19" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N19" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="O19" s="6">
         <v>0.7</v>
       </c>
-      <c r="Q19">
+      <c r="Q19" s="6">
         <v>3.2</v>
       </c>
-      <c r="R19">
+      <c r="R19" s="6">
         <v>150</v>
       </c>
-      <c r="S19">
+      <c r="S19" s="6">
         <f>($S$16-Q19)/(R19/1000)</f>
         <v>8.6666666666666661</v>
       </c>
-      <c r="V19" t="s">
-        <v>31</v>
-      </c>
-      <c r="W19">
+      <c r="V19" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="W19" s="6">
         <v>0.21</v>
       </c>
     </row>
     <row r="20" spans="12:23" x14ac:dyDescent="0.25">
-      <c r="M20" t="s">
-        <v>25</v>
-      </c>
-      <c r="N20" t="s">
-        <v>29</v>
-      </c>
-      <c r="O20">
+      <c r="M20" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N20" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="O20" s="6">
         <v>0.67</v>
       </c>
-      <c r="Q20">
+      <c r="Q20" s="6">
         <v>3.8</v>
       </c>
-      <c r="R20">
+      <c r="R20" s="6">
         <v>50</v>
       </c>
-      <c r="S20">
+      <c r="S20" s="6">
         <f>($S$16-Q20)/(R20/1000)</f>
         <v>14.000000000000004</v>
       </c>
-      <c r="V20" t="s">
-        <v>32</v>
-      </c>
-      <c r="W20">
+      <c r="V20" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="W20" s="6">
         <v>0.17699999999999999</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update bom; add alt regulator
</commit_message>
<xml_diff>
--- a/FlashlightBOM.xlsx
+++ b/FlashlightBOM.xlsx
@@ -2,29 +2,32 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chrisy\Documents\eagle\Flashlight\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28110" windowHeight="12135"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28125" windowHeight="12135"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
   <si>
     <t>Top pcb</t>
   </si>
@@ -126,6 +129,27 @@
   </si>
   <si>
     <t>Regulator</t>
+  </si>
+  <si>
+    <t>Current regulator</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>NSI50350ADT4GOSCT-ND</t>
+  </si>
+  <si>
+    <t>@10</t>
+  </si>
+  <si>
+    <t>@100</t>
+  </si>
+  <si>
+    <t>digikey</t>
+  </si>
+  <si>
+    <t>CW183-ND</t>
   </si>
 </sst>
 </file>
@@ -136,7 +160,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,6 +179,22 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -180,7 +220,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -190,15 +230,17 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -209,8 +251,11 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -269,7 +314,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -304,7 +349,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -489,19 +534,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W20"/>
+  <dimension ref="A1:W25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.28515625" style="6" customWidth="1"/>
-    <col min="2" max="5" width="9.140625" style="6"/>
+    <col min="2" max="5" width="8.85546875" style="6"/>
     <col min="6" max="6" width="12.28515625" style="6" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="6"/>
+    <col min="8" max="13" width="8.85546875" style="6"/>
+    <col min="14" max="14" width="21.85546875" style="6" customWidth="1"/>
+    <col min="15" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -610,6 +657,15 @@
       <c r="F5" s="6" t="s">
         <v>17</v>
       </c>
+      <c r="H5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" s="6">
+        <v>0.63</v>
+      </c>
       <c r="M5" s="6">
         <f>M4*2</f>
         <v>0</v>
@@ -884,8 +940,46 @@
         <v>0.17699999999999999</v>
       </c>
     </row>
+    <row r="23" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="L23" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="M24" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N24" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="O24" s="6">
+        <v>0.83</v>
+      </c>
+      <c r="P24" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="M25" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N25" s="9">
+        <v>1124300</v>
+      </c>
+      <c r="O25" s="6">
+        <v>0.111</v>
+      </c>
+      <c r="P25" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
bom updates - cleanup the bom
also add some misc items, like plastic bags, batteries
</commit_message>
<xml_diff>
--- a/FlashlightBOM.xlsx
+++ b/FlashlightBOM.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28125" windowHeight="12135"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="BOM" sheetId="1" r:id="rId1"/>
+    <sheet name="Regulator" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
   <si>
     <t>Top pcb</t>
   </si>
@@ -101,33 +102,12 @@
     <t>Solder lug</t>
   </si>
   <si>
-    <t>Mouser</t>
-  </si>
-  <si>
     <t>534-4002</t>
   </si>
   <si>
-    <t>889-SZ5M1WWC8V1V2FA</t>
-  </si>
-  <si>
     <t>941-MLEAWTA10002E7</t>
   </si>
   <si>
-    <t>941-CLP6BMKWCB0E0133</t>
-  </si>
-  <si>
-    <t>71-CRCW20104R30FKEF</t>
-  </si>
-  <si>
-    <t>71-CRCW20108R25FNEF</t>
-  </si>
-  <si>
-    <t>71-CRCW2010-14-E3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">or http://www.dx.com/p/aluminum-smooth-flashlight-reflector-silver-106488#.VC76FZ54rw9 </t>
-  </si>
-  <si>
     <t>Regulator</t>
   </si>
   <si>
@@ -149,19 +129,58 @@
     <t>digikey</t>
   </si>
   <si>
-    <t>CW183-ND</t>
-  </si>
-  <si>
     <t>mcmaster</t>
   </si>
   <si>
-    <t>4880K83</t>
-  </si>
-  <si>
     <t>Screws</t>
   </si>
   <si>
     <t>99461A105</t>
+  </si>
+  <si>
+    <t>ESD 3x4 resealable</t>
+  </si>
+  <si>
+    <t>Clear 3x4 resealable</t>
+  </si>
+  <si>
+    <t>amazon</t>
+  </si>
+  <si>
+    <t>Clear 5x6 resealable</t>
+  </si>
+  <si>
+    <t>CW182-ND</t>
+  </si>
+  <si>
+    <t>Alternative</t>
+  </si>
+  <si>
+    <t>C Cell</t>
+  </si>
+  <si>
+    <t>http://smile.amazon.com/ENERGIZER-ALKALINE-BATTERY-12-2024-later/dp/B00MOJ6GOE</t>
+  </si>
+  <si>
+    <t>charlotte 2101 1" female NPT coupler</t>
+  </si>
+  <si>
+    <t>http://smile.amazon.com/gp/product/B00P9045PC/</t>
+  </si>
+  <si>
+    <t>http://smile.amazon.com/gp/product/B009LIOOPO</t>
+  </si>
+  <si>
+    <t>http://smile.amazon.com/gp/product/B00LG07Q7I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://smile.amazon.com/DURACELL-PROCELL-Professional-Alkaline-Battery/dp/B00009V2QV </t>
+  </si>
+  <si>
+    <t>charlotte 1" schedule 40 PVC pipe (available in 2' lengths)</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/products/1684</t>
   </si>
 </sst>
 </file>
@@ -247,12 +266,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -264,10 +284,13 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -546,24 +569,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W25"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" style="6" customWidth="1"/>
     <col min="2" max="5" width="8.85546875" style="6"/>
     <col min="6" max="6" width="12.28515625" style="6" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="13" width="8.85546875" style="6"/>
+    <col min="8" max="8" width="10.42578125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="11" style="6" customWidth="1"/>
+    <col min="10" max="13" width="8.85546875" style="6"/>
     <col min="14" max="14" width="21.85546875" style="6" customWidth="1"/>
     <col min="15" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
@@ -583,8 +608,17 @@
       <c r="G1" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -603,7 +637,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -621,14 +655,10 @@
       <c r="F3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="6">
-        <f>4.55/3</f>
-        <v>1.5166666666666666</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B4" s="6">
         <v>1</v>
@@ -638,7 +668,7 @@
         <v>0.1109</v>
       </c>
       <c r="D4" s="8">
-        <f t="shared" ref="D4:D13" si="0">C4*B4</f>
+        <f t="shared" ref="D4:D17" si="0">C4*B4</f>
         <v>0.1109</v>
       </c>
       <c r="F4" s="6" t="s">
@@ -647,12 +677,9 @@
       <c r="G4" s="9">
         <v>1124300</v>
       </c>
-      <c r="M4" s="7">
-        <f>C2-M3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M4" s="7"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
@@ -669,8 +696,11 @@
       <c r="F5" s="6" t="s">
         <v>17</v>
       </c>
+      <c r="G5" s="12" t="s">
+        <v>50</v>
+      </c>
       <c r="H5" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>40</v>
@@ -678,12 +708,8 @@
       <c r="J5" s="6">
         <v>0.63</v>
       </c>
-      <c r="M5" s="6">
-        <f>M4*2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
@@ -701,10 +727,10 @@
         <v>16</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
@@ -722,8 +748,11 @@
       <c r="F7" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G7" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
@@ -745,7 +774,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
@@ -760,16 +789,13 @@
         <v>0.5</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
@@ -789,11 +815,9 @@
       <c r="G10" s="6">
         <v>1209700</v>
       </c>
-      <c r="I10" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="I10" s="12"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
@@ -814,7 +838,7 @@
         <v>1347100</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>23</v>
       </c>
@@ -822,34 +846,22 @@
         <v>2</v>
       </c>
       <c r="C12" s="8">
-        <v>0.113</v>
+        <v>0.183</v>
       </c>
       <c r="D12" s="8">
         <f t="shared" si="0"/>
-        <v>0.22600000000000001</v>
+        <v>0.36599999999999999</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>16</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="L12" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="M12" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="N12" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="O12" s="6">
-        <v>0.113</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B13" s="6">
         <v>2</v>
@@ -863,159 +875,189 @@
         <v>0.41560000000000002</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-    </row>
-    <row r="15" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="6">
+        <v>1</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.1598</v>
+      </c>
+      <c r="D14" s="8">
+        <f t="shared" si="0"/>
+        <v>0.1598</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="6">
+        <v>1</v>
+      </c>
+      <c r="C15" s="8">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D15" s="8">
+        <f t="shared" si="0"/>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="6">
+        <v>1</v>
+      </c>
+      <c r="C16" s="8">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="D16" s="8">
+        <f t="shared" si="0"/>
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="6">
+        <v>3</v>
+      </c>
+      <c r="C17" s="8">
+        <v>1</v>
+      </c>
+      <c r="D17" s="8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+    </row>
+    <row r="19" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="5">
-        <f>SUM(D2:D14)</f>
-        <v>8.1562454068241461</v>
-      </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S16" s="6">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="18" spans="12:23" x14ac:dyDescent="0.25">
-      <c r="L18" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="M18" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="N18" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="O18" s="6">
-        <v>0.78</v>
-      </c>
-      <c r="Q18" s="6">
-        <v>2.95</v>
-      </c>
-      <c r="R18" s="6">
-        <v>350</v>
-      </c>
-      <c r="S18" s="6">
-        <f>($S$16-Q18)/(R18/1000)</f>
-        <v>4.4285714285714279</v>
-      </c>
-      <c r="V18" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="W18" s="6">
-        <v>0.17699999999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="12:23" x14ac:dyDescent="0.25">
-      <c r="M19" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="N19" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="O19" s="6">
-        <v>0.7</v>
-      </c>
-      <c r="Q19" s="6">
-        <v>3.2</v>
-      </c>
-      <c r="R19" s="6">
-        <v>150</v>
-      </c>
-      <c r="S19" s="6">
-        <f>($S$16-Q19)/(R19/1000)</f>
-        <v>8.6666666666666661</v>
-      </c>
-      <c r="V19" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="W19" s="6">
-        <v>0.21</v>
-      </c>
-    </row>
-    <row r="20" spans="12:23" x14ac:dyDescent="0.25">
-      <c r="M20" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="N20" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="O20" s="6">
-        <v>0.67</v>
-      </c>
-      <c r="Q20" s="6">
-        <v>3.8</v>
-      </c>
-      <c r="R20" s="6">
-        <v>50</v>
-      </c>
-      <c r="S20" s="6">
-        <f>($S$16-Q20)/(R20/1000)</f>
-        <v>14.000000000000004</v>
-      </c>
-      <c r="V20" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="W20" s="6">
-        <v>0.17699999999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="12:23" x14ac:dyDescent="0.25">
-      <c r="L23" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="12:23" x14ac:dyDescent="0.25">
-      <c r="M24" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N24" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="O24" s="6">
-        <v>0.83</v>
-      </c>
-      <c r="P24" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="12:23" x14ac:dyDescent="0.25">
-      <c r="M25" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="N25" s="9">
-        <v>1124300</v>
-      </c>
-      <c r="O25" s="6">
-        <v>0.111</v>
-      </c>
-      <c r="P25" s="10" t="s">
-        <v>38</v>
-      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="5">
+        <f>SUM(D2:D18)</f>
+        <v>11.550045406824147</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G17" r:id="rId1"/>
+    <hyperlink ref="I17" r:id="rId2"/>
+    <hyperlink ref="G16" r:id="rId3"/>
+    <hyperlink ref="G15" r:id="rId4"/>
+    <hyperlink ref="G14" r:id="rId5"/>
+    <hyperlink ref="G5" r:id="rId6"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0.83</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="9">
+        <v>1124300</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0.111</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>